<commit_message>
Current state before implementing position 1 and 2 updates for processing station
</commit_message>
<xml_diff>
--- a/phieu-nhap-2025-06-21 (3).xlsx
+++ b/phieu-nhap-2025-06-21 (3).xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE17FCD4-685A-424D-B60B-35EDFCFD125F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Tiểu đoàn 2 - 20-06-2025" state="visible" r:id="rId4"/>
+    <sheet name="Tiểu đoàn 2 - 20-06-2025" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,11 +44,11 @@
     <t>TT</t>
   </si>
   <si>
-    <t xml:space="preserve">TÊN, QUI CÁCH,
+    <t>TÊN, QUI CÁCH,
 KÝ MÃ HIỆU VẬT TƯ</t>
   </si>
   <si>
-    <t xml:space="preserve">Đơn
+    <t>Đơn
 vị
 tính</t>
   </si>
@@ -103,28 +107,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,25 +156,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -175,10 +188,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,9 +541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -529,384 +557,383 @@
     <col min="7" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G2" s="3" t="s">
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>12</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="3">
         <v>12</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <v>14567</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>174804</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="9" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="6" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:H33"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:H6"/>
@@ -917,12 +944,13 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>